<commit_message>
- commented out the overly complex output directory creation - commented out dont overwrite outputs set to true from Reload failed jobs to test if the job will complete on the 2nd pass I commented out don’t overwrite outputs set to true step to see if the job will still continue to run with don’t overwrite ouputs as false After doing that the script still failed on the first pass but was successful on the second pass Also commented out the complex creation of folders
</commit_message>
<xml_diff>
--- a/autoast/2_jobs.xlsx
+++ b/autoast/2_jobs.xlsx
@@ -10,7 +10,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Domains" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -48,7 +48,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9D9D9"/>
+        <fgColor rgb="FFd9d9d9"/>
       </patternFill>
     </fill>
   </fills>
@@ -62,16 +62,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </left>
       <right style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -95,11 +95,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -109,16 +112,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
@@ -137,30 +139,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -235,13 +220,14 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:N3" headerRowCount="1" totalsRowShown="0">
+  <autoFilter ref="A1:N3"/>
   <tableColumns count="14">
     <tableColumn id="1" name="region" totalsRowLabel="Total"/>
     <tableColumn id="2" name="feature_layer"/>
     <tableColumn id="3" name="crown_file_number"/>
     <tableColumn id="4" name="disposition_number"/>
     <tableColumn id="5" name="parcel_number"/>
-    <tableColumn id="6" name="output_directory" dataDxfId="0"/>
+    <tableColumn id="6" name="output_directory"/>
     <tableColumn id="7" name="output_directory_same_as_input"/>
     <tableColumn id="8" name="dont_overwrite_outputs"/>
     <tableColumn id="9" name="skip_conflicts_and_constraints"/>
@@ -262,10 +248,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -303,71 +289,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -395,7 +381,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -418,11 +404,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -431,13 +417,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -447,7 +433,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -456,7 +442,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -465,7 +451,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -473,10 +459,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -548,66 +534,66 @@
   </sheetPr>
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="23.5703125" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
-    <col width="140.7109375" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
-    <col width="17.7109375" bestFit="1" customWidth="1" style="13" min="3" max="3"/>
-    <col width="16.85546875" bestFit="1" customWidth="1" style="13" min="4" max="4"/>
-    <col width="17.28515625" bestFit="1" customWidth="1" style="13" min="5" max="5"/>
-    <col width="110.42578125" bestFit="1" customWidth="1" style="19" min="6" max="6"/>
-    <col width="29.28515625" bestFit="1" customWidth="1" style="14" min="7" max="7"/>
-    <col width="29.140625" customWidth="1" style="14" min="8" max="8"/>
-    <col width="25.5703125" bestFit="1" customWidth="1" style="15" min="9" max="9"/>
-    <col width="21" bestFit="1" customWidth="1" style="15" min="10" max="10"/>
-    <col width="21.28515625" bestFit="1" customWidth="1" style="14" min="11" max="11"/>
-    <col width="13.7109375" bestFit="1" customWidth="1" style="14" min="12" max="12"/>
-    <col width="14.7109375" bestFit="1" customWidth="1" style="4" min="13" max="13"/>
-    <col width="11.5703125" bestFit="1" customWidth="1" style="16" min="14" max="14"/>
-    <col width="13.5703125" bestFit="1" customWidth="1" style="16" min="15" max="15"/>
+    <col width="23.57642857142857" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
+    <col width="140.7192857142857" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
+    <col width="17.71928571428571" bestFit="1" customWidth="1" style="13" min="3" max="3"/>
+    <col width="16.86214285714286" bestFit="1" customWidth="1" style="13" min="4" max="4"/>
+    <col width="17.29071428571428" bestFit="1" customWidth="1" style="13" min="5" max="5"/>
+    <col width="110.4335714285714" bestFit="1" customWidth="1" style="5" min="6" max="6"/>
+    <col width="29.29071428571428" bestFit="1" customWidth="1" style="14" min="7" max="7"/>
+    <col width="29.14785714285714" bestFit="1" customWidth="1" style="14" min="8" max="8"/>
+    <col width="25.57642857142857" bestFit="1" customWidth="1" style="14" min="9" max="9"/>
+    <col width="21.005" bestFit="1" customWidth="1" style="14" min="10" max="10"/>
+    <col width="21.29071428571428" bestFit="1" customWidth="1" style="14" min="11" max="11"/>
+    <col width="13.71928571428571" bestFit="1" customWidth="1" style="14" min="12" max="12"/>
+    <col width="14.71928571428571" bestFit="1" customWidth="1" style="5" min="13" max="13"/>
+    <col width="11.57642857142857" bestFit="1" customWidth="1" style="15" min="14" max="14"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="15" min="15" max="15"/>
   </cols>
   <sheetData>
-    <row r="1" ht="19.5" customHeight="1" s="5">
-      <c r="A1" s="2" t="inlineStr">
+    <row r="1" ht="19.5" customHeight="1">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>region</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>feature_layer</t>
         </is>
       </c>
-      <c r="C1" s="6" t="inlineStr">
+      <c r="C1" s="7" t="inlineStr">
         <is>
           <t>crown_file_number</t>
         </is>
       </c>
-      <c r="D1" s="6" t="inlineStr">
+      <c r="D1" s="7" t="inlineStr">
         <is>
           <t>disposition_number</t>
         </is>
       </c>
-      <c r="E1" s="6" t="inlineStr">
+      <c r="E1" s="7" t="inlineStr">
         <is>
           <t>parcel_number</t>
         </is>
       </c>
-      <c r="F1" s="17" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>output_directory</t>
         </is>
       </c>
-      <c r="G1" s="7" t="inlineStr">
+      <c r="G1" s="8" t="inlineStr">
         <is>
           <t>output_directory_same_as_input</t>
         </is>
       </c>
-      <c r="H1" s="7" t="inlineStr">
+      <c r="H1" s="8" t="inlineStr">
         <is>
           <t>dont_overwrite_outputs</t>
         </is>
@@ -622,17 +608,17 @@
           <t>suppress_map_creation</t>
         </is>
       </c>
-      <c r="K1" s="7" t="inlineStr">
+      <c r="K1" s="8" t="inlineStr">
         <is>
           <t>add_maps_to_current</t>
         </is>
       </c>
-      <c r="L1" s="7" t="inlineStr">
+      <c r="L1" s="8" t="inlineStr">
         <is>
           <t>run_as_fcbc</t>
         </is>
       </c>
-      <c r="M1" s="2" t="inlineStr">
+      <c r="M1" s="3" t="inlineStr">
         <is>
           <t>ast_condition</t>
         </is>
@@ -644,8 +630,8 @@
       </c>
       <c r="O1" s="9" t="n"/>
     </row>
-    <row r="2" ht="19.5" customHeight="1" s="5">
-      <c r="A2" s="2" t="inlineStr">
+    <row r="2" ht="19.5" customHeight="1">
+      <c r="A2" s="3" t="inlineStr">
         <is>
           <t>South_Coast</t>
         </is>
@@ -660,49 +646,51 @@
       <c r="E2" s="10" t="n">
         <v>968511</v>
       </c>
-      <c r="F2" s="18" t="inlineStr">
+      <c r="F2" s="11" t="inlineStr">
         <is>
           <t>\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\WildLifePermittingTest\AST_TEST\Parcel_968511</t>
         </is>
       </c>
-      <c r="G2" s="7" t="inlineStr">
+      <c r="G2" s="8" t="inlineStr">
         <is>
           <t>false</t>
         </is>
       </c>
-      <c r="H2" s="7" t="inlineStr">
+      <c r="H2" s="8" t="inlineStr">
         <is>
           <t>false</t>
         </is>
       </c>
-      <c r="I2" s="7" t="inlineStr">
+      <c r="I2" s="8" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J2" s="8" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="K2" s="8" t="inlineStr">
         <is>
           <t>false</t>
         </is>
       </c>
-      <c r="J2" s="7" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="K2" s="7" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="L2" s="7" t="b">
-        <v>1</v>
+      <c r="L2" s="8" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
       </c>
       <c r="M2" s="12" t="inlineStr">
         <is>
-          <t>Requeued</t>
-        </is>
-      </c>
-      <c r="N2" s="6" t="n"/>
-      <c r="O2" s="2" t="n"/>
-    </row>
-    <row r="3" ht="19.5" customHeight="1" s="5">
-      <c r="A3" s="2" t="inlineStr">
+          <t>COMPLETE</t>
+        </is>
+      </c>
+      <c r="N2" s="7" t="n"/>
+      <c r="O2" s="3" t="n"/>
+    </row>
+    <row r="3" ht="19.5" customHeight="1">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>Northeast</t>
         </is>
@@ -715,43 +703,44 @@
       <c r="C3" s="10" t="n"/>
       <c r="D3" s="10" t="n"/>
       <c r="E3" s="10" t="n"/>
-      <c r="F3" s="17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\WildLifePermittingTest\AST_TEST\876367
-</t>
-        </is>
-      </c>
-      <c r="G3" s="7" t="inlineStr">
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\WildLifePermittingTest\AST_TEST\Parcel_968511_v2</t>
+        </is>
+      </c>
+      <c r="G3" s="8" t="inlineStr">
         <is>
           <t>false</t>
         </is>
       </c>
-      <c r="H3" s="7" t="inlineStr">
+      <c r="H3" s="8" t="inlineStr">
         <is>
           <t>false</t>
         </is>
       </c>
-      <c r="I3" s="7" t="inlineStr">
+      <c r="I3" s="8" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J3" s="8" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="K3" s="8" t="inlineStr">
         <is>
           <t>false</t>
         </is>
       </c>
-      <c r="J3" s="7" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="K3" s="7" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="L3" s="7" t="b">
-        <v>1</v>
+      <c r="L3" s="8" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
       </c>
       <c r="M3" s="12" t="inlineStr">
         <is>
-          <t>Requeued</t>
+          <t>COMPLETE</t>
         </is>
       </c>
       <c r="N3" s="9" t="inlineStr">
@@ -763,7 +752,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
   <tableParts count="1">
     <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>
@@ -784,75 +772,90 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="27.140625" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
-    <col width="13.5703125" bestFit="1" customWidth="1" style="5" min="2" max="3"/>
+    <col width="27.14785714285714" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1" s="5">
+    <row r="1" ht="18.75" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Northeast</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="B1" s="6" t="n"/>
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="18.75" customHeight="1" s="5">
-      <c r="A2" s="2" t="inlineStr">
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="A2" s="3" t="inlineStr">
         <is>
           <t>Cariboo</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="B2" s="6" t="n"/>
+      <c r="C2" s="6" t="inlineStr">
         <is>
           <t>false</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="18.75" customHeight="1" s="5">
+    <row r="3" ht="18.75" customHeight="1">
       <c r="A3" s="1" t="inlineStr">
         <is>
           <t>Kootenay_Boundary</t>
         </is>
       </c>
-    </row>
-    <row r="4" ht="18.75" customHeight="1" s="5">
-      <c r="A4" s="2" t="inlineStr">
+      <c r="B3" s="6" t="n"/>
+      <c r="C3" s="6" t="n"/>
+    </row>
+    <row r="4" ht="18.75" customHeight="1">
+      <c r="A4" s="3" t="inlineStr">
         <is>
           <t>Skeena</t>
         </is>
       </c>
-    </row>
-    <row r="5" ht="18.75" customHeight="1" s="5">
+      <c r="B4" s="6" t="n"/>
+      <c r="C4" s="6" t="n"/>
+    </row>
+    <row r="5" ht="18.75" customHeight="1">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>South_Coast</t>
         </is>
       </c>
-    </row>
-    <row r="6" ht="18.75" customHeight="1" s="5">
-      <c r="A6" s="2" t="inlineStr">
+      <c r="B5" s="6" t="n"/>
+      <c r="C5" s="6" t="n"/>
+    </row>
+    <row r="6" ht="18.75" customHeight="1">
+      <c r="A6" s="3" t="inlineStr">
         <is>
           <t>Thompson_Okanagan</t>
         </is>
       </c>
-    </row>
-    <row r="7" ht="18.75" customHeight="1" s="5">
+      <c r="B6" s="6" t="n"/>
+      <c r="C6" s="6" t="n"/>
+    </row>
+    <row r="7" ht="18.75" customHeight="1">
       <c r="A7" s="1" t="inlineStr">
         <is>
           <t>West_Coast</t>
         </is>
       </c>
-    </row>
-    <row r="8" ht="18.75" customHeight="1" s="5">
-      <c r="A8" s="3" t="inlineStr">
+      <c r="B7" s="6" t="n"/>
+      <c r="C7" s="6" t="n"/>
+    </row>
+    <row r="8" ht="18.75" customHeight="1">
+      <c r="A8" s="4" t="inlineStr">
         <is>
           <t>Omineca</t>
         </is>
       </c>
+      <c r="B8" s="6" t="n"/>
+      <c r="C8" s="6" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- Deleted rebatch failed ast - Compared Reload failed jobs (seems to work) with load jobs (might be where initial pass was failing. * as a result of this moved Initialize dictionary into the for loops in load jobs And changed all ast_condition to Failed. The jobs ran successfully on the first pass.
So there is something about the 2nd pass that causes it to have success but not have success on the first pass.

Got as far as classifying input type in load jobs. Now will test again so I can isolate the fix rather than changing many things. Cut a pasted new load jobs back into old load jobs
</commit_message>
<xml_diff>
--- a/autoast/2_jobs.xlsx
+++ b/autoast/2_jobs.xlsx
@@ -95,7 +95,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
@@ -128,9 +128,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -542,19 +539,19 @@
   <cols>
     <col width="23.57642857142857" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
     <col width="140.7192857142857" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
-    <col width="17.71928571428571" bestFit="1" customWidth="1" style="13" min="3" max="3"/>
-    <col width="16.86214285714286" bestFit="1" customWidth="1" style="13" min="4" max="4"/>
-    <col width="17.29071428571428" bestFit="1" customWidth="1" style="13" min="5" max="5"/>
+    <col width="17.71928571428571" bestFit="1" customWidth="1" style="12" min="3" max="3"/>
+    <col width="16.86214285714286" bestFit="1" customWidth="1" style="12" min="4" max="4"/>
+    <col width="17.29071428571428" bestFit="1" customWidth="1" style="12" min="5" max="5"/>
     <col width="110.4335714285714" bestFit="1" customWidth="1" style="5" min="6" max="6"/>
-    <col width="29.29071428571428" bestFit="1" customWidth="1" style="14" min="7" max="7"/>
-    <col width="29.14785714285714" bestFit="1" customWidth="1" style="14" min="8" max="8"/>
-    <col width="25.57642857142857" bestFit="1" customWidth="1" style="14" min="9" max="9"/>
-    <col width="21.005" bestFit="1" customWidth="1" style="14" min="10" max="10"/>
-    <col width="21.29071428571428" bestFit="1" customWidth="1" style="14" min="11" max="11"/>
-    <col width="13.71928571428571" bestFit="1" customWidth="1" style="14" min="12" max="12"/>
+    <col width="29.29071428571428" bestFit="1" customWidth="1" style="13" min="7" max="7"/>
+    <col width="29.14785714285714" bestFit="1" customWidth="1" style="13" min="8" max="8"/>
+    <col width="25.57642857142857" bestFit="1" customWidth="1" style="13" min="9" max="9"/>
+    <col width="21.005" bestFit="1" customWidth="1" style="13" min="10" max="10"/>
+    <col width="21.29071428571428" bestFit="1" customWidth="1" style="13" min="11" max="11"/>
+    <col width="13.71928571428571" bestFit="1" customWidth="1" style="13" min="12" max="12"/>
     <col width="14.71928571428571" bestFit="1" customWidth="1" style="5" min="13" max="13"/>
-    <col width="11.57642857142857" bestFit="1" customWidth="1" style="15" min="14" max="14"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="15" min="15" max="15"/>
+    <col width="11.57642857142857" bestFit="1" customWidth="1" style="14" min="14" max="14"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="14" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1">
@@ -681,7 +678,7 @@
           <t>true</t>
         </is>
       </c>
-      <c r="M2" s="12" t="inlineStr">
+      <c r="M2" s="3" t="inlineStr">
         <is>
           <t>COMPLETE</t>
         </is>
@@ -738,7 +735,7 @@
           <t>true</t>
         </is>
       </c>
-      <c r="M3" s="12" t="inlineStr">
+      <c r="M3" s="3" t="inlineStr">
         <is>
           <t>COMPLETE</t>
         </is>

</xml_diff>

<commit_message>
- Moved Initialize dictionary in Load Jobs to outside the for loop - uncommented If current value of dont overwrite outputs to true - uncommented some of the main functions that were commented out for testing
</commit_message>
<xml_diff>
--- a/autoast/2_jobs.xlsx
+++ b/autoast/2_jobs.xlsx
@@ -95,7 +95,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
@@ -128,6 +128,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -539,19 +542,19 @@
   <cols>
     <col width="23.57642857142857" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
     <col width="140.7192857142857" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
-    <col width="17.71928571428571" bestFit="1" customWidth="1" style="12" min="3" max="3"/>
-    <col width="16.86214285714286" bestFit="1" customWidth="1" style="12" min="4" max="4"/>
-    <col width="17.29071428571428" bestFit="1" customWidth="1" style="12" min="5" max="5"/>
+    <col width="17.71928571428571" bestFit="1" customWidth="1" style="13" min="3" max="3"/>
+    <col width="16.86214285714286" bestFit="1" customWidth="1" style="13" min="4" max="4"/>
+    <col width="17.29071428571428" bestFit="1" customWidth="1" style="13" min="5" max="5"/>
     <col width="110.4335714285714" bestFit="1" customWidth="1" style="5" min="6" max="6"/>
-    <col width="29.29071428571428" bestFit="1" customWidth="1" style="13" min="7" max="7"/>
-    <col width="29.14785714285714" bestFit="1" customWidth="1" style="13" min="8" max="8"/>
-    <col width="25.57642857142857" bestFit="1" customWidth="1" style="13" min="9" max="9"/>
-    <col width="21.005" bestFit="1" customWidth="1" style="13" min="10" max="10"/>
-    <col width="21.29071428571428" bestFit="1" customWidth="1" style="13" min="11" max="11"/>
-    <col width="13.71928571428571" bestFit="1" customWidth="1" style="13" min="12" max="12"/>
+    <col width="29.29071428571428" bestFit="1" customWidth="1" style="14" min="7" max="7"/>
+    <col width="29.14785714285714" bestFit="1" customWidth="1" style="14" min="8" max="8"/>
+    <col width="25.57642857142857" bestFit="1" customWidth="1" style="14" min="9" max="9"/>
+    <col width="21.005" bestFit="1" customWidth="1" style="14" min="10" max="10"/>
+    <col width="21.29071428571428" bestFit="1" customWidth="1" style="14" min="11" max="11"/>
+    <col width="13.71928571428571" bestFit="1" customWidth="1" style="14" min="12" max="12"/>
     <col width="14.71928571428571" bestFit="1" customWidth="1" style="5" min="13" max="13"/>
-    <col width="11.57642857142857" bestFit="1" customWidth="1" style="14" min="14" max="14"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="14" min="15" max="15"/>
+    <col width="11.57642857142857" bestFit="1" customWidth="1" style="15" min="14" max="14"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="15" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1">
@@ -678,7 +681,7 @@
           <t>true</t>
         </is>
       </c>
-      <c r="M2" s="3" t="inlineStr">
+      <c r="M2" s="12" t="inlineStr">
         <is>
           <t>COMPLETE</t>
         </is>
@@ -735,7 +738,7 @@
           <t>true</t>
         </is>
       </c>
-      <c r="M3" s="3" t="inlineStr">
+      <c r="M3" s="12" t="inlineStr">
         <is>
           <t>COMPLETE</t>
         </is>

</xml_diff>

<commit_message>
Cleaned up imports in all of the submodules.
</commit_message>
<xml_diff>
--- a/autoast/2_jobs.xlsx
+++ b/autoast/2_jobs.xlsx
@@ -538,7 +538,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="23.57642857142857" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
     <col width="140.7192857142857" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
@@ -683,7 +683,7 @@
       </c>
       <c r="M2" s="12" t="inlineStr">
         <is>
-          <t>COMPLETE</t>
+          <t>Queued</t>
         </is>
       </c>
       <c r="N2" s="7" t="n"/>
@@ -740,7 +740,7 @@
       </c>
       <c r="M3" s="12" t="inlineStr">
         <is>
-          <t>COMPLETE</t>
+          <t>Queued</t>
         </is>
       </c>
       <c r="N3" s="9" t="inlineStr">
@@ -770,7 +770,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="27.14785714285714" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="2" max="2"/>

</xml_diff>